<commit_message>
asignación de autores Mat 9 tema 7
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion07/Escaleta_MA_09_07_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion07/Escaleta_MA_09_07_CO.xlsx
@@ -19,12 +19,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$P$1:$P$168</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateCount="2" iterateDelta="10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="181">
   <si>
     <t>Asignatura</t>
   </si>
@@ -554,6 +554,21 @@
   </si>
   <si>
     <t>Proponer entre 5 y 7 ecuaciones logaritmicas con sus posibles respuestas.</t>
+  </si>
+  <si>
+    <t>Johanna Vera</t>
+  </si>
+  <si>
+    <t>Alexander Rincón</t>
+  </si>
+  <si>
+    <t>Andrea Sabogal</t>
+  </si>
+  <si>
+    <t>Andrea Santos</t>
+  </si>
+  <si>
+    <t>Adriana Lasprilla</t>
   </si>
 </sst>
 </file>
@@ -609,7 +624,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -682,6 +697,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -710,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -811,21 +832,6 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -851,6 +857,24 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1159,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O18" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1174,114 +1198,114 @@
     <col min="7" max="7" width="74.5703125" style="28" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25" style="28" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="255.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="7.7109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="47.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25" style="28" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" style="2" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="2" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="6" style="2" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="10" style="2" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="255.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" style="2" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" style="2" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="47.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="71.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" style="2"/>
+    <col min="22" max="22" width="12.7109375" style="2" customWidth="1"/>
     <col min="23" max="23" width="93.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="24" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="K1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="36"/>
-      <c r="O1" s="37" t="s">
+      <c r="N1" s="45"/>
+      <c r="O1" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="37" t="s">
+      <c r="P1" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="Q1" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="R1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="38" t="s">
+      <c r="S1" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="T1" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="35" t="s">
+      <c r="U1" s="44" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="40"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="39"/>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="34"/>
       <c r="M2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="35"/>
-    </row>
-    <row r="3" spans="1:21" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="44"/>
+    </row>
+    <row r="3" spans="1:22" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1339,8 +1363,11 @@
       <c r="U3" s="17" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.2">
+      <c r="V3" s="48" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1398,8 +1425,11 @@
       <c r="U4" s="17" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V4" s="48" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1450,7 +1480,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -1508,8 +1538,11 @@
       <c r="U6" s="17" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.2">
+      <c r="V6" s="48" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1565,8 +1598,11 @@
       <c r="U7" s="17" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V7" s="48" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -1621,7 +1657,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -1674,7 +1710,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1732,8 +1768,11 @@
       <c r="U10" s="17" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V10" s="48" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -1786,7 +1825,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1842,8 +1881,11 @@
       <c r="U12" s="17" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" ht="15" x14ac:dyDescent="0.2">
+      <c r="V12" s="48" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -1901,8 +1943,11 @@
       <c r="U13" s="17" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V13" s="48" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
@@ -1955,7 +2000,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -2014,7 +2059,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -2072,6 +2117,9 @@
       <c r="U16" s="17" t="s">
         <v>156</v>
       </c>
+      <c r="V16" s="48" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="17" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
@@ -2130,6 +2178,9 @@
       </c>
       <c r="U17" s="17" t="s">
         <v>158</v>
+      </c>
+      <c r="V17" s="48" t="s">
+        <v>180</v>
       </c>
       <c r="W17" s="3" t="s">
         <v>17</v>
@@ -2246,6 +2297,9 @@
       <c r="U19" s="17" t="s">
         <v>158</v>
       </c>
+      <c r="V19" s="48" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
@@ -2356,6 +2410,9 @@
       <c r="U21" s="33" t="s">
         <v>158</v>
       </c>
+      <c r="V21" s="48" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
@@ -2523,6 +2580,9 @@
       <c r="U24" s="17" t="s">
         <v>158</v>
       </c>
+      <c r="V24" s="48" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
@@ -2688,6 +2748,9 @@
       <c r="U27" s="17" t="s">
         <v>158</v>
       </c>
+      <c r="V27" s="48" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
@@ -2802,6 +2865,9 @@
       <c r="U29" s="17" t="s">
         <v>158</v>
       </c>
+      <c r="V29" s="48" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="30" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
@@ -2859,6 +2925,9 @@
       <c r="U30" s="17" t="s">
         <v>158</v>
       </c>
+      <c r="V30" s="48" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="31" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
@@ -2917,6 +2986,9 @@
       </c>
       <c r="U31" s="17" t="s">
         <v>158</v>
+      </c>
+      <c r="V31" s="48" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="15" x14ac:dyDescent="0.2">
@@ -2972,7 +3044,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
@@ -3025,7 +3097,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>16</v>
       </c>
@@ -3066,7 +3138,7 @@
       <c r="T34" s="24"/>
       <c r="U34" s="25"/>
     </row>
-    <row r="35" spans="1:21" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>16</v>
       </c>
@@ -3122,8 +3194,9 @@
       <c r="U35" s="17" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" ht="15" x14ac:dyDescent="0.2">
+      <c r="V35" s="48"/>
+    </row>
+    <row r="36" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>16</v>
       </c>
@@ -3177,8 +3250,9 @@
       <c r="U36" s="17" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V36" s="48"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G41" s="29"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -3190,7 +3264,7 @@
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G42" s="29"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
@@ -3202,7 +3276,7 @@
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G43" s="29"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -3214,7 +3288,7 @@
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G44" s="29"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
@@ -3226,7 +3300,7 @@
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G45" s="29"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -3238,7 +3312,7 @@
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G46" s="29"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -3250,7 +3324,7 @@
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G47" s="29"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -3262,7 +3336,7 @@
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G48" s="29"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
@@ -4786,6 +4860,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -4798,14 +4880,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N36">

</xml_diff>

<commit_message>
Material enviado por autores
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion07/Escaleta_MA_09_07_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion07/Escaleta_MA_09_07_CO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="187">
   <si>
     <t>Asignatura</t>
   </si>
@@ -569,6 +569,24 @@
   </si>
   <si>
     <t>Identifica características de las gráficas de funciones exponenciales</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Esta el recurso, falta solicitud gráfica</t>
+  </si>
+  <si>
+    <t>No está</t>
+  </si>
+  <si>
+    <t>Bloqueado autor</t>
+  </si>
+  <si>
+    <t>Vacio</t>
+  </si>
+  <si>
+    <t>Solo tiene 2 preguntas</t>
   </si>
 </sst>
 </file>
@@ -705,7 +723,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -838,6 +856,21 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -863,21 +896,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1190,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W168"/>
+  <dimension ref="A1:X168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1224,97 +1242,97 @@
     <col min="24" max="16384" width="11.453125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="46" t="s">
+      <c r="N1" s="36"/>
+      <c r="O1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="46" t="s">
+      <c r="P1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="Q1" s="44" t="s">
+      <c r="Q1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="43" t="s">
+      <c r="R1" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="47" t="s">
+      <c r="S1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="43" t="s">
+      <c r="T1" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="44" t="s">
+      <c r="U1" s="35" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="35"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="34"/>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" s="40"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="44"/>
-    </row>
-    <row r="3" spans="1:22" s="2" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="35"/>
+    </row>
+    <row r="3" spans="1:23" s="2" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1375,8 +1393,11 @@
       <c r="V3" s="33" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="W3" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1437,8 +1458,11 @@
       <c r="V4" s="33" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W4" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1488,8 +1512,11 @@
       <c r="U5" s="24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="W5" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -1550,8 +1577,11 @@
       <c r="V6" s="33" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="W6" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1610,8 +1640,11 @@
       <c r="V7" s="33" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W7" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -1665,8 +1698,11 @@
       <c r="U8" s="24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W8" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -1718,8 +1754,11 @@
       <c r="U9" s="24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="W9" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1780,8 +1819,11 @@
       <c r="V10" s="33" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W10" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -1833,8 +1875,11 @@
       <c r="U11" s="24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="W11" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1893,8 +1938,11 @@
       <c r="V12" s="33" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="W12" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -1955,8 +2003,11 @@
       <c r="V13" s="33" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W13" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
@@ -2008,8 +2059,11 @@
       <c r="U14" s="24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W14" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -2067,8 +2121,11 @@
       <c r="U15" s="24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="W15" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -2129,8 +2186,11 @@
       <c r="V16" s="33" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="W16" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -2192,10 +2252,13 @@
         <v>179</v>
       </c>
       <c r="W17" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="X17" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -2210,7 +2273,7 @@
       </c>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="49" t="s">
         <v>99</v>
       </c>
       <c r="H18" s="8">
@@ -2247,8 +2310,11 @@
       <c r="U18" s="24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="W18" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
@@ -2309,8 +2375,11 @@
       <c r="V19" s="33" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W19" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
@@ -2362,8 +2431,11 @@
       <c r="U20" s="24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W20" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -2422,8 +2494,11 @@
       <c r="V21" s="33" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W21" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>16</v>
       </c>
@@ -2475,8 +2550,11 @@
       <c r="U22" s="24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W22" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>16</v>
       </c>
@@ -2530,8 +2608,11 @@
       <c r="U23" s="24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="W23" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>16</v>
       </c>
@@ -2592,8 +2673,11 @@
       <c r="V24" s="33" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W24" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>16</v>
       </c>
@@ -2647,8 +2731,11 @@
       <c r="U25" s="24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W25" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -2700,8 +2787,11 @@
       <c r="U26" s="24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="W26" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>16</v>
       </c>
@@ -2760,8 +2850,11 @@
       <c r="V27" s="33" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W27" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>16</v>
       </c>
@@ -2817,8 +2910,11 @@
       <c r="U28" s="24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="W28" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
@@ -2877,8 +2973,11 @@
       <c r="V29" s="33" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="30" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="W29" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>16</v>
       </c>
@@ -2937,8 +3036,11 @@
       <c r="V30" s="33" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="W30" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>16</v>
       </c>
@@ -2999,8 +3101,11 @@
       <c r="V31" s="33" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="32" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="W31" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>16</v>
       </c>
@@ -3053,7 +3158,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
@@ -3106,7 +3211,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>16</v>
       </c>
@@ -3147,7 +3252,7 @@
       <c r="T34" s="23"/>
       <c r="U34" s="24"/>
     </row>
-    <row r="35" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>16</v>
       </c>
@@ -3204,8 +3309,11 @@
         <v>157</v>
       </c>
       <c r="V35" s="33"/>
-    </row>
-    <row r="36" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="W35" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>16</v>
       </c>
@@ -3260,8 +3368,11 @@
         <v>157</v>
       </c>
       <c r="V36" s="33"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W36" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="G41" s="28"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -3273,7 +3384,7 @@
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="G42" s="28"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
@@ -3285,7 +3396,7 @@
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="G43" s="28"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -3297,7 +3408,7 @@
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="G44" s="28"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
@@ -3309,7 +3420,7 @@
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="G45" s="28"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -3321,7 +3432,7 @@
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="G46" s="28"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -3333,7 +3444,7 @@
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="G47" s="28"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -3345,7 +3456,7 @@
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="G48" s="28"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
@@ -4869,14 +4980,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -4889,6 +4992,14 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N36">

</xml_diff>

<commit_message>
Cuaderno de estudio MA_09_07_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion07/Escaleta_MA_09_07_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion07/Escaleta_MA_09_07_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CristhianAndres\Documents\Github\Matematicas\fuentes\contenidos\grado09\guion07\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CristhianAndres\Documents\GitHub\Matematicas\fuentes\contenidos\grado09\guion07\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -325,9 +325,6 @@
     <t>Proponer expresiones donde se empleen las propiedades de los logaritmos para escribirlos como un solo logarítmo.</t>
   </si>
   <si>
-    <t>Practica el calculo del logaritmo</t>
-  </si>
-  <si>
     <t>Practica el cálculo de logaritmos</t>
   </si>
   <si>
@@ -569,6 +566,9 @@
   </si>
   <si>
     <t>Identifica características de las gráficas de funciones exponenciales</t>
+  </si>
+  <si>
+    <t>Practica el cálculo del logaritmo</t>
   </si>
 </sst>
 </file>
@@ -839,6 +839,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -864,27 +885,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1192,129 +1192,129 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="E19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="74.54296875" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.90625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="74.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="2" customWidth="1"/>
     <col min="10" max="10" width="25" style="27" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="2" customWidth="1"/>
-    <col min="12" max="12" width="11.7265625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="7.90625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="21.54296875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="23.26953125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="22.1796875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="14.7265625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="21.54296875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="37.453125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="71.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.7265625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="93.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="11.453125" style="3"/>
+    <col min="12" max="12" width="11.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="23.28515625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="22.140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="37.42578125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="71.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="93.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="F1" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="G1" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="G1" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="40" t="s">
+      <c r="I1" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="J1" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="38"/>
+      <c r="O1" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="J1" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="46" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q1" s="44" t="s">
+      <c r="Q1" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="43" t="s">
+      <c r="R1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="47" t="s">
+      <c r="S1" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="43" t="s">
+      <c r="T1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="44" t="s">
+      <c r="U1" s="37" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="35"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="34"/>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="42"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="41"/>
       <c r="M2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="44"/>
-    </row>
-    <row r="3" spans="1:22" s="2" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="37"/>
+    </row>
+    <row r="3" spans="1:22" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1325,11 +1325,11 @@
         <v>36</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="34" t="s">
         <v>59</v>
       </c>
       <c r="H3" s="8">
@@ -1364,19 +1364,19 @@
         <v>32</v>
       </c>
       <c r="S3" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="T3" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="T3" s="17" t="s">
+      <c r="U3" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="U3" s="16" t="s">
-        <v>155</v>
-      </c>
       <c r="V3" s="33" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1387,11 +1387,11 @@
         <v>36</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="19" t="s">
         <v>61</v>
       </c>
       <c r="H4" s="20">
@@ -1426,19 +1426,19 @@
         <v>33</v>
       </c>
       <c r="S4" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T4" s="17" t="s">
         <v>53</v>
       </c>
       <c r="U4" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V4" s="33" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1449,12 +1449,12 @@
         <v>36</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
-      <c r="G5" s="49" t="s">
-        <v>180</v>
+      <c r="G5" s="19" t="s">
+        <v>179</v>
       </c>
       <c r="H5" s="20">
         <v>3</v>
@@ -1464,7 +1464,7 @@
         <v>65</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="1"/>
@@ -1489,7 +1489,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -1500,11 +1500,11 @@
         <v>36</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
-      <c r="G6" s="49" t="s">
+      <c r="G6" s="19" t="s">
         <v>73</v>
       </c>
       <c r="H6" s="8">
@@ -1539,19 +1539,19 @@
         <v>33</v>
       </c>
       <c r="S6" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="T6" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="T6" s="17" t="s">
+      <c r="U6" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="U6" s="16" t="s">
-        <v>160</v>
-      </c>
       <c r="V6" s="33" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1562,11 +1562,11 @@
         <v>36</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
-      <c r="G7" s="49" t="s">
+      <c r="G7" s="19" t="s">
         <v>79</v>
       </c>
       <c r="H7" s="8">
@@ -1599,19 +1599,19 @@
         <v>33</v>
       </c>
       <c r="S7" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T7" s="17" t="s">
         <v>55</v>
       </c>
       <c r="U7" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V7" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -1622,13 +1622,13 @@
         <v>36</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>34</v>
       </c>
       <c r="F8" s="18"/>
-      <c r="G8" s="49" t="s">
+      <c r="G8" s="19" t="s">
         <v>81</v>
       </c>
       <c r="H8" s="20">
@@ -1638,10 +1638,10 @@
         <v>37</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L8" s="9"/>
       <c r="M8" s="1"/>
@@ -1666,7 +1666,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -1677,24 +1677,24 @@
         <v>36</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
-      <c r="G9" s="49" t="s">
+      <c r="G9" s="19" t="s">
         <v>49</v>
       </c>
       <c r="H9" s="20">
         <v>7</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>69</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L9" s="9"/>
       <c r="M9" s="1"/>
@@ -1719,7 +1719,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1730,11 +1730,11 @@
         <v>36</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
-      <c r="G10" s="49" t="s">
+      <c r="G10" s="19" t="s">
         <v>72</v>
       </c>
       <c r="H10" s="8">
@@ -1769,19 +1769,19 @@
         <v>33</v>
       </c>
       <c r="S10" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T10" s="17" t="s">
         <v>54</v>
       </c>
       <c r="U10" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V10" s="33" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -1792,24 +1792,24 @@
         <v>36</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
-      <c r="G11" s="49" t="s">
+      <c r="G11" s="19" t="s">
         <v>70</v>
       </c>
       <c r="H11" s="8">
         <v>9</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J11" s="10" t="s">
         <v>71</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L11" s="9"/>
       <c r="M11" s="1"/>
@@ -1834,7 +1834,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1845,12 +1845,12 @@
         <v>36</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
-      <c r="G12" s="49" t="s">
-        <v>102</v>
+      <c r="G12" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="H12" s="20">
         <v>10</v>
@@ -1859,7 +1859,7 @@
         <v>37</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K12" s="11" t="s">
         <v>37</v>
@@ -1870,7 +1870,7 @@
         <v>24</v>
       </c>
       <c r="O12" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P12" s="13" t="s">
         <v>31</v>
@@ -1882,19 +1882,19 @@
         <v>33</v>
       </c>
       <c r="S12" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="T12" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="U12" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="T12" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="U12" s="16" t="s">
-        <v>157</v>
-      </c>
       <c r="V12" s="33" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -1905,11 +1905,11 @@
         <v>36</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
-      <c r="G13" s="49" t="s">
+      <c r="G13" s="19" t="s">
         <v>75</v>
       </c>
       <c r="H13" s="20">
@@ -1919,7 +1919,7 @@
         <v>37</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K13" s="11" t="s">
         <v>37</v>
@@ -1944,19 +1944,19 @@
         <v>33</v>
       </c>
       <c r="S13" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="T13" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="U13" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="T13" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="U13" s="16" t="s">
-        <v>157</v>
-      </c>
       <c r="V13" s="33" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
@@ -1967,12 +1967,12 @@
         <v>36</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
-      <c r="G14" s="49" t="s">
-        <v>148</v>
+      <c r="G14" s="19" t="s">
+        <v>147</v>
       </c>
       <c r="H14" s="8">
         <v>12</v>
@@ -1984,7 +1984,7 @@
         <v>77</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="1"/>
@@ -2009,7 +2009,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -2020,14 +2020,14 @@
         <v>36</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>34</v>
       </c>
       <c r="F15" s="18"/>
-      <c r="G15" s="49" t="s">
-        <v>104</v>
+      <c r="G15" s="19" t="s">
+        <v>103</v>
       </c>
       <c r="H15" s="8">
         <v>13</v>
@@ -2039,7 +2039,7 @@
         <v>82</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L15" s="9" t="s">
         <v>19</v>
@@ -2062,13 +2062,13 @@
         <v>67</v>
       </c>
       <c r="T15" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="U15" s="24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -2083,14 +2083,14 @@
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
-      <c r="G16" s="49" t="s">
+      <c r="G16" s="19" t="s">
         <v>84</v>
       </c>
       <c r="H16" s="20">
         <v>14</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J16" s="10" t="s">
         <v>85</v>
@@ -2118,19 +2118,19 @@
         <v>32</v>
       </c>
       <c r="S16" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T16" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="U16" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="V16" s="33" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
-      <c r="G17" s="49" t="s">
+      <c r="G17" s="19" t="s">
         <v>86</v>
       </c>
       <c r="H17" s="20">
@@ -2180,22 +2180,22 @@
         <v>33</v>
       </c>
       <c r="S17" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="T17" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="U17" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="T17" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="U17" s="16" t="s">
-        <v>157</v>
-      </c>
       <c r="V17" s="33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="W17" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -2210,8 +2210,8 @@
       </c>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
-      <c r="G18" s="19" t="s">
-        <v>99</v>
+      <c r="G18" s="35" t="s">
+        <v>180</v>
       </c>
       <c r="H18" s="8">
         <v>16</v>
@@ -2220,10 +2220,10 @@
         <v>37</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="1"/>
@@ -2242,13 +2242,13 @@
         <v>67</v>
       </c>
       <c r="T18" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U18" s="24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
@@ -2263,7 +2263,7 @@
       </c>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
-      <c r="G19" s="49" t="s">
+      <c r="G19" s="19" t="s">
         <v>88</v>
       </c>
       <c r="H19" s="8">
@@ -2298,19 +2298,19 @@
         <v>33</v>
       </c>
       <c r="S19" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T19" s="17" t="s">
         <v>57</v>
       </c>
       <c r="U19" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V19" s="33" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
@@ -2325,20 +2325,20 @@
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
-      <c r="G20" s="49" t="s">
+      <c r="G20" s="19" t="s">
         <v>90</v>
       </c>
       <c r="H20" s="20">
         <v>18</v>
       </c>
       <c r="I20" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>91</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L20" s="9"/>
       <c r="M20" s="1"/>
@@ -2363,7 +2363,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -2378,8 +2378,8 @@
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
-      <c r="G21" s="49" t="s">
-        <v>110</v>
+      <c r="G21" s="19" t="s">
+        <v>109</v>
       </c>
       <c r="H21" s="20">
         <v>19</v>
@@ -2388,7 +2388,7 @@
         <v>37</v>
       </c>
       <c r="J21" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K21" s="11" t="s">
         <v>37</v>
@@ -2399,7 +2399,7 @@
         <v>26</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P21" s="13" t="s">
         <v>31</v>
@@ -2411,19 +2411,19 @@
         <v>33</v>
       </c>
       <c r="S21" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="T21" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="U21" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="T21" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="U21" s="32" t="s">
-        <v>157</v>
-      </c>
       <c r="V21" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>16</v>
       </c>
@@ -2438,7 +2438,7 @@
       </c>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
-      <c r="G22" s="49" t="s">
+      <c r="G22" s="19" t="s">
         <v>93</v>
       </c>
       <c r="H22" s="8">
@@ -2451,7 +2451,7 @@
         <v>92</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L22" s="9"/>
       <c r="M22" s="1"/>
@@ -2476,7 +2476,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>16</v>
       </c>
@@ -2491,7 +2491,7 @@
       </c>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
-      <c r="G23" s="49" t="s">
+      <c r="G23" s="19" t="s">
         <v>95</v>
       </c>
       <c r="H23" s="8">
@@ -2504,7 +2504,7 @@
         <v>96</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L23" s="9" t="s">
         <v>19</v>
@@ -2531,7 +2531,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>16</v>
       </c>
@@ -2546,8 +2546,8 @@
       </c>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
-      <c r="G24" s="49" t="s">
-        <v>105</v>
+      <c r="G24" s="19" t="s">
+        <v>104</v>
       </c>
       <c r="H24" s="20">
         <v>22</v>
@@ -2581,19 +2581,19 @@
         <v>33</v>
       </c>
       <c r="S24" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="T24" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="U24" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="T24" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="U24" s="16" t="s">
-        <v>157</v>
-      </c>
       <c r="V24" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>16</v>
       </c>
@@ -2610,8 +2610,8 @@
         <v>34</v>
       </c>
       <c r="F25" s="18"/>
-      <c r="G25" s="49" t="s">
-        <v>106</v>
+      <c r="G25" s="19" t="s">
+        <v>105</v>
       </c>
       <c r="H25" s="20">
         <v>23</v>
@@ -2620,10 +2620,10 @@
         <v>37</v>
       </c>
       <c r="J25" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L25" s="9"/>
       <c r="M25" s="1"/>
@@ -2642,13 +2642,13 @@
         <v>67</v>
       </c>
       <c r="T25" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U25" s="24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -2659,24 +2659,24 @@
         <v>36</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
-      <c r="G26" s="49" t="s">
+      <c r="G26" s="19" t="s">
         <v>51</v>
       </c>
       <c r="H26" s="8">
         <v>24</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J26" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L26" s="9"/>
       <c r="M26" s="1"/>
@@ -2695,13 +2695,13 @@
         <v>67</v>
       </c>
       <c r="T26" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U26" s="24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>16</v>
       </c>
@@ -2712,12 +2712,12 @@
         <v>36</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
-      <c r="G27" s="49" t="s">
-        <v>112</v>
+      <c r="G27" s="19" t="s">
+        <v>111</v>
       </c>
       <c r="H27" s="8">
         <v>25</v>
@@ -2726,7 +2726,7 @@
         <v>37</v>
       </c>
       <c r="J27" s="25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K27" s="11" t="s">
         <v>37</v>
@@ -2737,7 +2737,7 @@
         <v>25</v>
       </c>
       <c r="O27" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P27" s="13" t="s">
         <v>31</v>
@@ -2749,19 +2749,19 @@
         <v>33</v>
       </c>
       <c r="S27" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T27" s="17" t="s">
         <v>56</v>
       </c>
       <c r="U27" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V27" s="33" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>16</v>
       </c>
@@ -2772,14 +2772,14 @@
         <v>36</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>34</v>
       </c>
       <c r="F28" s="18"/>
-      <c r="G28" s="49" t="s">
-        <v>108</v>
+      <c r="G28" s="19" t="s">
+        <v>107</v>
       </c>
       <c r="H28" s="20">
         <v>26</v>
@@ -2791,7 +2791,7 @@
         <v>45</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L28" s="9" t="s">
         <v>19</v>
@@ -2812,13 +2812,13 @@
         <v>67</v>
       </c>
       <c r="T28" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U28" s="24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
@@ -2833,8 +2833,8 @@
       </c>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
-      <c r="G29" s="49" t="s">
-        <v>114</v>
+      <c r="G29" s="19" t="s">
+        <v>113</v>
       </c>
       <c r="H29" s="20">
         <v>27</v>
@@ -2843,7 +2843,7 @@
         <v>37</v>
       </c>
       <c r="J29" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K29" s="11" t="s">
         <v>37</v>
@@ -2854,7 +2854,7 @@
         <v>25</v>
       </c>
       <c r="O29" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P29" s="13" t="s">
         <v>31</v>
@@ -2866,19 +2866,19 @@
         <v>33</v>
       </c>
       <c r="S29" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="T29" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="U29" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="T29" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="U29" s="16" t="s">
-        <v>157</v>
-      </c>
       <c r="V29" s="33" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>16</v>
       </c>
@@ -2893,8 +2893,8 @@
       </c>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
-      <c r="G30" s="49" t="s">
-        <v>115</v>
+      <c r="G30" s="19" t="s">
+        <v>114</v>
       </c>
       <c r="H30" s="8">
         <v>28</v>
@@ -2903,7 +2903,7 @@
         <v>37</v>
       </c>
       <c r="J30" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K30" s="11" t="s">
         <v>37</v>
@@ -2914,7 +2914,7 @@
         <v>25</v>
       </c>
       <c r="O30" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P30" s="13" t="s">
         <v>31</v>
@@ -2926,19 +2926,19 @@
         <v>33</v>
       </c>
       <c r="S30" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="T30" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="U30" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="T30" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="U30" s="16" t="s">
-        <v>157</v>
-      </c>
       <c r="V30" s="33" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>16</v>
       </c>
@@ -2953,8 +2953,8 @@
       </c>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="49" t="s">
-        <v>118</v>
+      <c r="G31" s="19" t="s">
+        <v>117</v>
       </c>
       <c r="H31" s="8">
         <v>29</v>
@@ -2963,7 +2963,7 @@
         <v>37</v>
       </c>
       <c r="J31" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K31" s="11" t="s">
         <v>37</v>
@@ -2988,19 +2988,19 @@
         <v>33</v>
       </c>
       <c r="S31" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="T31" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="U31" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="T31" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="U31" s="16" t="s">
-        <v>157</v>
-      </c>
       <c r="V31" s="33" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" ht="14.5" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>16</v>
       </c>
@@ -3011,12 +3011,12 @@
         <v>36</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
-      <c r="G32" s="49" t="s">
-        <v>120</v>
+      <c r="G32" s="19" t="s">
+        <v>119</v>
       </c>
       <c r="H32" s="20">
         <v>30</v>
@@ -3025,10 +3025,10 @@
         <v>37</v>
       </c>
       <c r="J32" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K32" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L32" s="9"/>
       <c r="M32" s="1"/>
@@ -3047,13 +3047,13 @@
         <v>67</v>
       </c>
       <c r="T32" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U32" s="24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
@@ -3064,12 +3064,12 @@
         <v>36</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
-      <c r="G33" s="49" t="s">
-        <v>121</v>
+      <c r="G33" s="19" t="s">
+        <v>120</v>
       </c>
       <c r="H33" s="20">
         <v>31</v>
@@ -3078,10 +3078,10 @@
         <v>37</v>
       </c>
       <c r="J33" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K33" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L33" s="9"/>
       <c r="M33" s="1"/>
@@ -3100,13 +3100,13 @@
         <v>67</v>
       </c>
       <c r="T33" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="U33" s="24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>16</v>
       </c>
@@ -3117,19 +3117,19 @@
         <v>36</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
       <c r="G34" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H34" s="8">
         <v>32</v>
       </c>
       <c r="I34" s="21"/>
       <c r="J34" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K34" s="11" t="s">
         <v>37</v>
@@ -3147,7 +3147,7 @@
       <c r="T34" s="23"/>
       <c r="U34" s="24"/>
     </row>
-    <row r="35" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>16</v>
       </c>
@@ -3158,12 +3158,12 @@
         <v>36</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
       <c r="G35" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H35" s="8">
         <v>33</v>
@@ -3172,7 +3172,7 @@
         <v>37</v>
       </c>
       <c r="J35" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K35" s="11" t="s">
         <v>37</v>
@@ -3183,7 +3183,7 @@
         <v>24</v>
       </c>
       <c r="O35" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P35" s="13" t="s">
         <v>31</v>
@@ -3195,17 +3195,17 @@
         <v>33</v>
       </c>
       <c r="S35" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T35" s="17" t="s">
         <v>58</v>
       </c>
       <c r="U35" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V35" s="33"/>
     </row>
-    <row r="36" spans="1:22" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>16</v>
       </c>
@@ -3216,12 +3216,12 @@
         <v>36</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H36" s="20">
         <v>34</v>
@@ -3230,7 +3230,7 @@
         <v>37</v>
       </c>
       <c r="J36" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K36" s="11" t="s">
         <v>37</v>
@@ -3242,7 +3242,7 @@
       </c>
       <c r="O36" s="12"/>
       <c r="P36" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q36" s="14">
         <v>6</v>
@@ -3251,17 +3251,17 @@
         <v>33</v>
       </c>
       <c r="S36" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="T36" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="U36" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="T36" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="U36" s="16" t="s">
-        <v>157</v>
-      </c>
       <c r="V36" s="33"/>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G41" s="28"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -3273,7 +3273,7 @@
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G42" s="28"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
@@ -3285,7 +3285,7 @@
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G43" s="28"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -3297,7 +3297,7 @@
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G44" s="28"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
@@ -3309,7 +3309,7 @@
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G45" s="28"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -3321,7 +3321,7 @@
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G46" s="28"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -3333,7 +3333,7 @@
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G47" s="28"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -3345,7 +3345,7 @@
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G48" s="28"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
@@ -3357,7 +3357,7 @@
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
     </row>
-    <row r="49" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="7:16" x14ac:dyDescent="0.2">
       <c r="G49" s="28"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
@@ -3369,7 +3369,7 @@
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
     </row>
-    <row r="50" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="7:16" x14ac:dyDescent="0.2">
       <c r="G50" s="28"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
@@ -3381,7 +3381,7 @@
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
     </row>
-    <row r="51" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="7:16" x14ac:dyDescent="0.2">
       <c r="G51" s="28"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
@@ -3393,7 +3393,7 @@
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
     </row>
-    <row r="52" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="7:16" x14ac:dyDescent="0.2">
       <c r="G52" s="28"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
@@ -3405,7 +3405,7 @@
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
     </row>
-    <row r="53" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="7:16" x14ac:dyDescent="0.2">
       <c r="G53" s="28"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
@@ -3417,7 +3417,7 @@
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
     </row>
-    <row r="54" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="7:16" x14ac:dyDescent="0.2">
       <c r="G54" s="28"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
@@ -3429,7 +3429,7 @@
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
     </row>
-    <row r="56" spans="7:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="7:16" x14ac:dyDescent="0.2">
       <c r="G56" s="28"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
@@ -3441,73 +3441,73 @@
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
     </row>
-    <row r="77" spans="13:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="13:16" x14ac:dyDescent="0.2">
       <c r="M77" s="3"/>
       <c r="N77" s="3"/>
       <c r="O77" s="3"/>
       <c r="P77" s="3"/>
     </row>
-    <row r="79" spans="13:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="13:16" x14ac:dyDescent="0.2">
       <c r="M79" s="3"/>
       <c r="N79" s="3"/>
       <c r="O79" s="3"/>
       <c r="P79" s="3"/>
     </row>
-    <row r="80" spans="13:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="13:16" x14ac:dyDescent="0.2">
       <c r="M80" s="3"/>
       <c r="N80" s="3"/>
       <c r="O80" s="3"/>
       <c r="P80" s="3"/>
     </row>
-    <row r="81" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:16" x14ac:dyDescent="0.2">
       <c r="M81" s="3"/>
       <c r="N81" s="3"/>
       <c r="O81" s="3"/>
       <c r="P81" s="3"/>
     </row>
-    <row r="82" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:16" x14ac:dyDescent="0.2">
       <c r="M82" s="3"/>
       <c r="N82" s="3"/>
       <c r="O82" s="3"/>
       <c r="P82" s="3"/>
     </row>
-    <row r="83" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:16" x14ac:dyDescent="0.2">
       <c r="M83" s="3"/>
       <c r="N83" s="3"/>
       <c r="O83" s="3"/>
       <c r="P83" s="3"/>
     </row>
-    <row r="84" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:16" x14ac:dyDescent="0.2">
       <c r="M84" s="3"/>
       <c r="N84" s="3"/>
       <c r="O84" s="3"/>
       <c r="P84" s="3"/>
     </row>
-    <row r="85" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:16" x14ac:dyDescent="0.2">
       <c r="M85" s="3"/>
       <c r="N85" s="3"/>
       <c r="O85" s="3"/>
       <c r="P85" s="3"/>
     </row>
-    <row r="86" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:16" x14ac:dyDescent="0.2">
       <c r="M86" s="3"/>
       <c r="N86" s="3"/>
       <c r="O86" s="3"/>
       <c r="P86" s="3"/>
     </row>
-    <row r="87" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:16" x14ac:dyDescent="0.2">
       <c r="M87" s="3"/>
       <c r="N87" s="3"/>
       <c r="O87" s="3"/>
       <c r="P87" s="3"/>
     </row>
-    <row r="88" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:16" x14ac:dyDescent="0.2">
       <c r="M88" s="3"/>
       <c r="N88" s="3"/>
       <c r="O88" s="3"/>
       <c r="P88" s="3"/>
     </row>
-    <row r="89" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="28"/>
@@ -3524,7 +3524,7 @@
       <c r="O89" s="3"/>
       <c r="P89" s="3"/>
     </row>
-    <row r="90" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="28"/>
@@ -3541,7 +3541,7 @@
       <c r="O90" s="3"/>
       <c r="P90" s="3"/>
     </row>
-    <row r="91" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="28"/>
@@ -3558,7 +3558,7 @@
       <c r="O91" s="3"/>
       <c r="P91" s="3"/>
     </row>
-    <row r="92" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="28"/>
@@ -3575,7 +3575,7 @@
       <c r="O92" s="3"/>
       <c r="P92" s="3"/>
     </row>
-    <row r="93" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="28"/>
@@ -3592,7 +3592,7 @@
       <c r="O93" s="3"/>
       <c r="P93" s="3"/>
     </row>
-    <row r="94" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="28"/>
@@ -3609,7 +3609,7 @@
       <c r="O94" s="3"/>
       <c r="P94" s="3"/>
     </row>
-    <row r="95" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" s="28"/>
@@ -3626,7 +3626,7 @@
       <c r="O95" s="3"/>
       <c r="P95" s="3"/>
     </row>
-    <row r="96" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="28"/>
@@ -3643,7 +3643,7 @@
       <c r="O96" s="3"/>
       <c r="P96" s="3"/>
     </row>
-    <row r="97" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
       <c r="D97" s="28"/>
@@ -3660,7 +3660,7 @@
       <c r="O97" s="3"/>
       <c r="P97" s="3"/>
     </row>
-    <row r="98" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" s="28"/>
@@ -3677,7 +3677,7 @@
       <c r="O98" s="3"/>
       <c r="P98" s="3"/>
     </row>
-    <row r="99" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
       <c r="D99" s="28"/>
@@ -3694,7 +3694,7 @@
       <c r="O99" s="3"/>
       <c r="P99" s="3"/>
     </row>
-    <row r="100" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="28"/>
@@ -3711,7 +3711,7 @@
       <c r="O100" s="3"/>
       <c r="P100" s="3"/>
     </row>
-    <row r="101" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="28"/>
@@ -3728,7 +3728,7 @@
       <c r="O101" s="3"/>
       <c r="P101" s="3"/>
     </row>
-    <row r="102" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="28"/>
@@ -3745,7 +3745,7 @@
       <c r="O102" s="3"/>
       <c r="P102" s="3"/>
     </row>
-    <row r="103" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="28"/>
@@ -3762,7 +3762,7 @@
       <c r="O103" s="3"/>
       <c r="P103" s="3"/>
     </row>
-    <row r="104" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
       <c r="D104" s="28"/>
@@ -3779,7 +3779,7 @@
       <c r="O104" s="3"/>
       <c r="P104" s="3"/>
     </row>
-    <row r="105" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="D105" s="28"/>
@@ -3796,7 +3796,7 @@
       <c r="O105" s="3"/>
       <c r="P105" s="3"/>
     </row>
-    <row r="106" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="28"/>
@@ -3813,7 +3813,7 @@
       <c r="O106" s="3"/>
       <c r="P106" s="3"/>
     </row>
-    <row r="107" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" s="28"/>
@@ -3830,7 +3830,7 @@
       <c r="O107" s="3"/>
       <c r="P107" s="3"/>
     </row>
-    <row r="108" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" s="28"/>
@@ -3847,7 +3847,7 @@
       <c r="O108" s="3"/>
       <c r="P108" s="3"/>
     </row>
-    <row r="109" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="28"/>
@@ -3864,7 +3864,7 @@
       <c r="O109" s="3"/>
       <c r="P109" s="3"/>
     </row>
-    <row r="110" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="28"/>
@@ -3881,7 +3881,7 @@
       <c r="O110" s="3"/>
       <c r="P110" s="3"/>
     </row>
-    <row r="111" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="28"/>
@@ -3898,7 +3898,7 @@
       <c r="O111" s="3"/>
       <c r="P111" s="3"/>
     </row>
-    <row r="112" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="28"/>
@@ -3915,7 +3915,7 @@
       <c r="O112" s="3"/>
       <c r="P112" s="3"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" s="28"/>
@@ -3932,7 +3932,7 @@
       <c r="O113" s="3"/>
       <c r="P113" s="3"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
       <c r="D114" s="28"/>
@@ -3949,7 +3949,7 @@
       <c r="O114" s="3"/>
       <c r="P114" s="3"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
       <c r="D115" s="28"/>
@@ -3966,7 +3966,7 @@
       <c r="O115" s="3"/>
       <c r="P115" s="3"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
       <c r="D116" s="28"/>
@@ -3983,7 +3983,7 @@
       <c r="O116" s="3"/>
       <c r="P116" s="3"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
       <c r="D117" s="28"/>
@@ -4000,7 +4000,7 @@
       <c r="O117" s="3"/>
       <c r="P117" s="3"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
       <c r="D118" s="28"/>
@@ -4017,7 +4017,7 @@
       <c r="O118" s="3"/>
       <c r="P118" s="3"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
       <c r="D119" s="28"/>
@@ -4034,7 +4034,7 @@
       <c r="O119" s="3"/>
       <c r="P119" s="3"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
       <c r="D120" s="28"/>
@@ -4051,7 +4051,7 @@
       <c r="O120" s="3"/>
       <c r="P120" s="3"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
       <c r="D121" s="28"/>
@@ -4068,7 +4068,7 @@
       <c r="O121" s="3"/>
       <c r="P121" s="3"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" s="28"/>
@@ -4085,7 +4085,7 @@
       <c r="O122" s="3"/>
       <c r="P122" s="3"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
       <c r="D123" s="28"/>
@@ -4102,7 +4102,7 @@
       <c r="O123" s="3"/>
       <c r="P123" s="3"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="28"/>
@@ -4119,7 +4119,7 @@
       <c r="O124" s="3"/>
       <c r="P124" s="3"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="28"/>
@@ -4136,7 +4136,7 @@
       <c r="O125" s="3"/>
       <c r="P125" s="3"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" s="28"/>
@@ -4153,7 +4153,7 @@
       <c r="O126" s="3"/>
       <c r="P126" s="3"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
       <c r="D127" s="28"/>
@@ -4170,7 +4170,7 @@
       <c r="O127" s="3"/>
       <c r="P127" s="3"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
       <c r="D128" s="28"/>
@@ -4187,7 +4187,7 @@
       <c r="O128" s="3"/>
       <c r="P128" s="3"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
       <c r="D129" s="28"/>
@@ -4204,7 +4204,7 @@
       <c r="O129" s="3"/>
       <c r="P129" s="3"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
       <c r="D130" s="28"/>
@@ -4221,7 +4221,7 @@
       <c r="O130" s="3"/>
       <c r="P130" s="3"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
       <c r="D131" s="28"/>
@@ -4238,7 +4238,7 @@
       <c r="O131" s="3"/>
       <c r="P131" s="3"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
       <c r="D132" s="28"/>
@@ -4255,7 +4255,7 @@
       <c r="O132" s="3"/>
       <c r="P132" s="3"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
       <c r="D133" s="28"/>
@@ -4272,7 +4272,7 @@
       <c r="O133" s="3"/>
       <c r="P133" s="3"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
       <c r="D134" s="28"/>
@@ -4289,7 +4289,7 @@
       <c r="O134" s="3"/>
       <c r="P134" s="3"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
       <c r="D135" s="28"/>
@@ -4306,7 +4306,7 @@
       <c r="O135" s="3"/>
       <c r="P135" s="3"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
       <c r="D136" s="28"/>
@@ -4323,7 +4323,7 @@
       <c r="O136" s="3"/>
       <c r="P136" s="3"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
       <c r="D137" s="28"/>
@@ -4340,7 +4340,7 @@
       <c r="O137" s="3"/>
       <c r="P137" s="3"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
       <c r="D138" s="28"/>
@@ -4357,7 +4357,7 @@
       <c r="O138" s="3"/>
       <c r="P138" s="3"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
       <c r="D139" s="28"/>
@@ -4374,7 +4374,7 @@
       <c r="O139" s="3"/>
       <c r="P139" s="3"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
       <c r="D140" s="28"/>
@@ -4391,7 +4391,7 @@
       <c r="O140" s="3"/>
       <c r="P140" s="3"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
       <c r="D141" s="28"/>
@@ -4408,7 +4408,7 @@
       <c r="O141" s="3"/>
       <c r="P141" s="3"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
       <c r="D142" s="28"/>
@@ -4425,7 +4425,7 @@
       <c r="O142" s="3"/>
       <c r="P142" s="3"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
       <c r="D143" s="28"/>
@@ -4442,7 +4442,7 @@
       <c r="O143" s="3"/>
       <c r="P143" s="3"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
       <c r="D144" s="28"/>
@@ -4459,7 +4459,7 @@
       <c r="O144" s="3"/>
       <c r="P144" s="3"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
       <c r="D145" s="28"/>
@@ -4476,7 +4476,7 @@
       <c r="O145" s="3"/>
       <c r="P145" s="3"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
       <c r="D146" s="28"/>
@@ -4493,7 +4493,7 @@
       <c r="O146" s="3"/>
       <c r="P146" s="3"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
       <c r="D147" s="28"/>
@@ -4510,7 +4510,7 @@
       <c r="O147" s="3"/>
       <c r="P147" s="3"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
       <c r="D148" s="28"/>
@@ -4527,7 +4527,7 @@
       <c r="O148" s="3"/>
       <c r="P148" s="3"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
       <c r="D149" s="28"/>
@@ -4544,7 +4544,7 @@
       <c r="O149" s="3"/>
       <c r="P149" s="3"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
       <c r="D150" s="28"/>
@@ -4561,7 +4561,7 @@
       <c r="O150" s="3"/>
       <c r="P150" s="3"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
       <c r="D151" s="28"/>
@@ -4578,7 +4578,7 @@
       <c r="O151" s="3"/>
       <c r="P151" s="3"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
       <c r="D152" s="28"/>
@@ -4595,7 +4595,7 @@
       <c r="O152" s="3"/>
       <c r="P152" s="3"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
       <c r="D153" s="28"/>
@@ -4612,7 +4612,7 @@
       <c r="O153" s="3"/>
       <c r="P153" s="3"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
       <c r="D154" s="28"/>
@@ -4629,7 +4629,7 @@
       <c r="O154" s="3"/>
       <c r="P154" s="3"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
       <c r="D155" s="28"/>
@@ -4646,7 +4646,7 @@
       <c r="O155" s="3"/>
       <c r="P155" s="3"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
       <c r="D156" s="28"/>
@@ -4663,7 +4663,7 @@
       <c r="O156" s="3"/>
       <c r="P156" s="3"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
       <c r="D157" s="28"/>
@@ -4680,7 +4680,7 @@
       <c r="O157" s="3"/>
       <c r="P157" s="3"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
       <c r="D158" s="28"/>
@@ -4697,7 +4697,7 @@
       <c r="O158" s="3"/>
       <c r="P158" s="3"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
       <c r="D159" s="28"/>
@@ -4714,7 +4714,7 @@
       <c r="O159" s="3"/>
       <c r="P159" s="3"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
       <c r="D160" s="28"/>
@@ -4731,7 +4731,7 @@
       <c r="O160" s="3"/>
       <c r="P160" s="3"/>
     </row>
-    <row r="161" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
       <c r="D161" s="28"/>
@@ -4748,7 +4748,7 @@
       <c r="O161" s="3"/>
       <c r="P161" s="3"/>
     </row>
-    <row r="162" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
       <c r="D162" s="28"/>
@@ -4765,7 +4765,7 @@
       <c r="O162" s="3"/>
       <c r="P162" s="3"/>
     </row>
-    <row r="163" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
       <c r="D163" s="28"/>
@@ -4782,7 +4782,7 @@
       <c r="O163" s="3"/>
       <c r="P163" s="3"/>
     </row>
-    <row r="164" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
       <c r="D164" s="28"/>
@@ -4799,7 +4799,7 @@
       <c r="O164" s="3"/>
       <c r="P164" s="3"/>
     </row>
-    <row r="165" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
       <c r="D165" s="28"/>
@@ -4816,7 +4816,7 @@
       <c r="O165" s="3"/>
       <c r="P165" s="3"/>
     </row>
-    <row r="166" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
       <c r="D166" s="28"/>
@@ -4833,7 +4833,7 @@
       <c r="O166" s="3"/>
       <c r="P166" s="3"/>
     </row>
-    <row r="167" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
       <c r="D167" s="28"/>
@@ -4850,7 +4850,7 @@
       <c r="O167" s="3"/>
       <c r="P167" s="3"/>
     </row>
-    <row r="168" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
       <c r="D168" s="28"/>
@@ -4869,14 +4869,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -4889,6 +4881,14 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N36">
@@ -4918,7 +4918,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4930,7 +4930,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>